<commit_message>
test push from personal comp
</commit_message>
<xml_diff>
--- a/Booz_financials_2022.xlsx
+++ b/Booz_financials_2022.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dduff\Documents\Budgeting\Investing\Financial-Projects\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C13440F4-3394-46C6-8813-BFB7ED2C99E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="1470" yWindow="1470" windowWidth="16875" windowHeight="10523" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Balance_Sheet" sheetId="1" r:id="rId1"/>
@@ -12,7 +18,7 @@
     <sheet name="Comprehensive_Income" sheetId="3" r:id="rId3"/>
     <sheet name="Cash_Flows" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -667,8 +673,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -731,6 +737,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -777,7 +791,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -809,9 +823,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -843,6 +875,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1018,14 +1068,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="3" max="3" width="11.9296875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1057,12 +1112,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -1097,7 +1152,7 @@
         <v>350384000</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -1108,7 +1163,7 @@
         <v>1411894</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -1137,7 +1192,7 @@
         <v>84142</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
@@ -1172,7 +1227,7 @@
         <v>1424352000</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
@@ -1207,7 +1262,7 @@
         <v>166570000</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
@@ -1221,7 +1276,7 @@
         <v>240122</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
@@ -1256,7 +1311,7 @@
         <v>236220000</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
@@ -1291,7 +1346,7 @@
         <v>1277369000</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
@@ -1326,7 +1381,7 @@
         <v>62985000</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>20</v>
       </c>
@@ -1361,7 +1416,7 @@
         <v>3177528000</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>21</v>
       </c>
@@ -1390,7 +1445,7 @@
         <v>1029586000</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>22</v>
       </c>
@@ -1398,7 +1453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
         <v>23</v>
       </c>
@@ -1418,7 +1473,7 @@
         <v>10032000</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>24</v>
       </c>
@@ -1429,7 +1484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
         <v>25</v>
       </c>
@@ -1437,7 +1492,7 @@
         <v>49559</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
         <v>26</v>
       </c>
@@ -1445,7 +1500,7 @@
         <v>29129000</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
         <v>27</v>
       </c>
@@ -1453,7 +1508,7 @@
         <v>5689000</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
         <v>28</v>
       </c>
@@ -1461,12 +1516,12 @@
         <v>9564000</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
         <v>30</v>
       </c>
@@ -1501,7 +1556,7 @@
         <v>55562000</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
         <v>31</v>
       </c>
@@ -1536,7 +1591,7 @@
         <v>451065000</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
         <v>32</v>
       </c>
@@ -1571,7 +1626,7 @@
         <v>385433000</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
         <v>33</v>
       </c>
@@ -1585,7 +1640,7 @@
         <v>49021</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
         <v>34</v>
       </c>
@@ -1620,7 +1675,7 @@
         <v>62300000</v>
       </c>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
         <v>35</v>
       </c>
@@ -1655,7 +1710,7 @@
         <v>964646000</v>
       </c>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
         <v>36</v>
       </c>
@@ -1690,7 +1745,7 @@
         <v>1659611000</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="s">
         <v>37</v>
       </c>
@@ -1704,7 +1759,7 @@
         <v>270266</v>
       </c>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="s">
         <v>38</v>
       </c>
@@ -1724,7 +1779,7 @@
         <v>4485</v>
       </c>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="s">
         <v>39</v>
       </c>
@@ -1759,7 +1814,7 @@
         <v>269460000</v>
       </c>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A32" s="1" t="s">
         <v>40</v>
       </c>
@@ -1794,17 +1849,17 @@
         <v>2950735000</v>
       </c>
     </row>
-    <row r="33" spans="1:11">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A33" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="34" spans="1:11">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A34" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="35" spans="1:11">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A35" s="1" t="s">
         <v>43</v>
       </c>
@@ -1824,12 +1879,12 @@
         <v>57018000</v>
       </c>
     </row>
-    <row r="36" spans="1:11">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A36" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="37" spans="1:11">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A37" s="1" t="s">
         <v>45</v>
       </c>
@@ -1843,12 +1898,12 @@
         <v>58444</v>
       </c>
     </row>
-    <row r="38" spans="1:11">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A38" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="39" spans="1:11">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A39" s="1" t="s">
         <v>47</v>
       </c>
@@ -1862,7 +1917,7 @@
         <v>10286000</v>
       </c>
     </row>
-    <row r="40" spans="1:11">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A40" s="1" t="s">
         <v>48</v>
       </c>
@@ -1870,12 +1925,12 @@
         <v>8231</v>
       </c>
     </row>
-    <row r="41" spans="1:11">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A41" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="42" spans="1:11">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A42" s="1" t="s">
         <v>50</v>
       </c>
@@ -1886,7 +1941,7 @@
         <v>1629</v>
       </c>
     </row>
-    <row r="43" spans="1:11">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A43" s="1" t="s">
         <v>51</v>
       </c>
@@ -1897,7 +1952,7 @@
         <v>-1216163</v>
       </c>
     </row>
-    <row r="44" spans="1:11">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A44" s="1" t="s">
         <v>52</v>
       </c>
@@ -1932,7 +1987,7 @@
         <v>120836000</v>
       </c>
     </row>
-    <row r="45" spans="1:11">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A45" s="1" t="s">
         <v>53</v>
       </c>
@@ -1967,7 +2022,7 @@
         <v>124775000</v>
       </c>
     </row>
-    <row r="46" spans="1:11">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A46" s="1" t="s">
         <v>54</v>
       </c>
@@ -1975,7 +2030,7 @@
         <v>8585</v>
       </c>
     </row>
-    <row r="47" spans="1:11">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A47" s="1" t="s">
         <v>55</v>
       </c>
@@ -1983,7 +2038,7 @@
         <v>1046070</v>
       </c>
     </row>
-    <row r="48" spans="1:11">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A48" s="1" t="s">
         <v>56</v>
       </c>
@@ -1991,7 +2046,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="49" spans="1:11">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A49" s="1" t="s">
         <v>57</v>
       </c>
@@ -2011,7 +2066,7 @@
         <v>554628</v>
       </c>
     </row>
-    <row r="50" spans="1:11">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A50" s="1" t="s">
         <v>58</v>
       </c>
@@ -2031,7 +2086,7 @@
         <v>3603366</v>
       </c>
     </row>
-    <row r="51" spans="1:11">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A51" s="1" t="s">
         <v>59</v>
       </c>
@@ -2063,7 +2118,7 @@
         <v>-13787000</v>
       </c>
     </row>
-    <row r="52" spans="1:11">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A52" s="1" t="s">
         <v>60</v>
       </c>
@@ -2071,7 +2126,7 @@
         <v>1613</v>
       </c>
     </row>
-    <row r="53" spans="1:11">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A53" s="1" t="s">
         <v>61</v>
       </c>
@@ -2079,7 +2134,7 @@
         <v>-898095</v>
       </c>
     </row>
-    <row r="54" spans="1:11">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A54" s="1" t="s">
         <v>62</v>
       </c>
@@ -2087,7 +2142,7 @@
         <v>1599</v>
       </c>
     </row>
-    <row r="55" spans="1:11">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A55" s="1" t="s">
         <v>63</v>
       </c>
@@ -2095,7 +2150,7 @@
         <v>-711450</v>
       </c>
     </row>
-    <row r="56" spans="1:11">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A56" s="1" t="s">
         <v>64</v>
       </c>
@@ -2103,7 +2158,7 @@
         <v>1580</v>
       </c>
     </row>
-    <row r="57" spans="1:11">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A57" s="1" t="s">
         <v>65</v>
       </c>
@@ -2111,12 +2166,12 @@
         <v>-461457</v>
       </c>
     </row>
-    <row r="58" spans="1:11">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A58" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="59" spans="1:11">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A59" s="1" t="s">
         <v>67</v>
       </c>
@@ -2124,7 +2179,7 @@
         <v>-191900</v>
       </c>
     </row>
-    <row r="60" spans="1:11">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A60" s="1" t="s">
         <v>68</v>
       </c>
@@ -2138,7 +2193,7 @@
         <v>186498</v>
       </c>
     </row>
-    <row r="61" spans="1:11">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A61" s="1" t="s">
         <v>69</v>
       </c>
@@ -2158,12 +2213,12 @@
         <v>3177528000</v>
       </c>
     </row>
-    <row r="62" spans="1:11">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A62" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="63" spans="1:11">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A63" s="1" t="s">
         <v>71</v>
       </c>
@@ -2174,7 +2229,7 @@
         <v>-72293</v>
       </c>
     </row>
-    <row r="64" spans="1:11">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A64" s="1" t="s">
         <v>72</v>
       </c>
@@ -2182,7 +2237,7 @@
         <v>-10153</v>
       </c>
     </row>
-    <row r="65" spans="1:11">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A65" s="1" t="s">
         <v>73</v>
       </c>
@@ -2193,7 +2248,7 @@
         <v>226793000</v>
       </c>
     </row>
-    <row r="66" spans="1:11">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A66" s="1" t="s">
         <v>74</v>
       </c>
@@ -2201,12 +2256,12 @@
         <v>-6444000</v>
       </c>
     </row>
-    <row r="67" spans="1:11">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A67" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="68" spans="1:11">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A68" s="1" t="s">
         <v>76</v>
       </c>
@@ -2226,22 +2281,22 @@
         <v>1364000</v>
       </c>
     </row>
-    <row r="69" spans="1:11">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A69" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="70" spans="1:11">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A70" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="71" spans="1:11">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A71" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="72" spans="1:11">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A72" s="1" t="s">
         <v>80</v>
       </c>
@@ -2258,17 +2313,17 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="73" spans="1:11">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A73" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="74" spans="1:11">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A74" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="75" spans="1:11">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A75" s="1" t="s">
         <v>83</v>
       </c>
@@ -2282,17 +2337,17 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="76" spans="1:11">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A76" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="77" spans="1:11">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A77" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="78" spans="1:11">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A78" s="1" t="s">
         <v>86</v>
       </c>
@@ -2312,14 +2367,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2351,12 +2406,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>88</v>
       </c>
@@ -2391,12 +2446,12 @@
         <v>5758059</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>90</v>
       </c>
@@ -2431,7 +2486,7 @@
         <v>2871240</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>91</v>
       </c>
@@ -2466,7 +2521,7 @@
         <v>1532590</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>92</v>
       </c>
@@ -2501,7 +2556,7 @@
         <v>833986</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>93</v>
       </c>
@@ -2536,7 +2591,7 @@
         <v>74009</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>94</v>
       </c>
@@ -2571,7 +2626,7 @@
         <v>5311825</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>95</v>
       </c>
@@ -2606,7 +2661,7 @@
         <v>446234</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>96</v>
       </c>
@@ -2641,7 +2696,7 @@
         <v>-70284</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>97</v>
       </c>
@@ -2658,7 +2713,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>98</v>
       </c>
@@ -2693,7 +2748,7 @@
         <v>368311</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>99</v>
       </c>
@@ -2728,7 +2783,7 @@
         <v>149253</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
         <v>100</v>
       </c>
@@ -2763,7 +2818,7 @@
         <v>219058</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>101</v>
       </c>
@@ -2771,7 +2826,7 @@
         <v>-163</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
         <v>102</v>
       </c>
@@ -2779,7 +2834,7 @@
         <v>466740</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
         <v>103</v>
       </c>
@@ -2787,7 +2842,7 @@
         <v>-10662</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
         <v>104</v>
       </c>
@@ -2807,7 +2862,7 @@
         <v>-7639</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
         <v>105</v>
       </c>
@@ -2818,12 +2873,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
         <v>107</v>
       </c>
@@ -2858,7 +2913,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
         <v>108</v>
       </c>
@@ -2893,12 +2948,12 @@
         <v>145</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
         <v>110</v>
       </c>
@@ -2912,14 +2967,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2936,12 +2991,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>112</v>
       </c>
@@ -2961,27 +3016,27 @@
         <v>305111</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>117</v>
       </c>
@@ -2998,7 +3053,7 @@
         <v>-7971</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>118</v>
       </c>
@@ -3018,7 +3073,7 @@
         <v>-171</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>119</v>
       </c>
@@ -3038,7 +3093,7 @@
         <v>4822</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>120</v>
       </c>
@@ -3058,17 +3113,17 @@
         <v>309933</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>123</v>
       </c>
@@ -3082,14 +3137,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:K95"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3121,12 +3176,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>112</v>
       </c>
@@ -3161,12 +3216,12 @@
         <v>219058</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>93</v>
       </c>
@@ -3201,7 +3256,7 @@
         <v>74009</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>126</v>
       </c>
@@ -3215,7 +3270,7 @@
         <v>55096</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>127</v>
       </c>
@@ -3250,7 +3305,7 @@
         <v>24841</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>47</v>
       </c>
@@ -3285,7 +3340,7 @@
         <v>48088</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>128</v>
       </c>
@@ -3296,7 +3351,7 @@
         <v>4395</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>129</v>
       </c>
@@ -3307,7 +3362,7 @@
         <v>13239</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>130</v>
       </c>
@@ -3315,7 +3370,7 @@
         <v>-3388</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>131</v>
       </c>
@@ -3323,7 +3378,7 @@
         <v>-12759</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>132</v>
       </c>
@@ -3331,7 +3386,7 @@
         <v>-3322</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>133</v>
       </c>
@@ -3357,7 +3412,7 @@
         <v>17224</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
         <v>134</v>
       </c>
@@ -3365,7 +3420,7 @@
         <v>1772</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>135</v>
       </c>
@@ -3382,7 +3437,7 @@
         <v>-31924</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
         <v>136</v>
       </c>
@@ -3393,7 +3448,7 @@
         <v>-246</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
         <v>137</v>
       </c>
@@ -3410,7 +3465,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
         <v>138</v>
       </c>
@@ -3424,7 +3479,7 @@
         <v>-26860</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
         <v>139</v>
       </c>
@@ -3438,7 +3493,7 @@
         <v>-254</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
         <v>140</v>
       </c>
@@ -3446,7 +3501,7 @@
         <v>11682</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
         <v>141</v>
       </c>
@@ -3454,12 +3509,12 @@
         <v>1106</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
         <v>143</v>
       </c>
@@ -3470,7 +3525,7 @@
         <v>47081</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
         <v>144</v>
       </c>
@@ -3505,7 +3560,7 @@
         <v>104877</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
         <v>145</v>
       </c>
@@ -3513,7 +3568,7 @@
         <v>-19489</v>
       </c>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
         <v>146</v>
       </c>
@@ -3548,7 +3603,7 @@
         <v>-26832</v>
       </c>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
         <v>147</v>
       </c>
@@ -3583,7 +3638,7 @@
         <v>-23760</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="s">
         <v>148</v>
       </c>
@@ -3591,7 +3646,7 @@
         <v>-27588</v>
       </c>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="s">
         <v>149</v>
       </c>
@@ -3626,7 +3681,7 @@
         <v>464654</v>
       </c>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="s">
         <v>150</v>
       </c>
@@ -3655,7 +3710,7 @@
         <v>-5923</v>
       </c>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A32" s="1" t="s">
         <v>151</v>
       </c>
@@ -3687,7 +3742,7 @@
         <v>2723</v>
       </c>
     </row>
-    <row r="33" spans="1:11">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A33" s="1" t="s">
         <v>152</v>
       </c>
@@ -3719,7 +3774,7 @@
         <v>-11367</v>
       </c>
     </row>
-    <row r="34" spans="1:11">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A34" s="1" t="s">
         <v>153</v>
       </c>
@@ -3730,7 +3785,7 @@
         <v>-37651</v>
       </c>
     </row>
-    <row r="35" spans="1:11">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A35" s="1" t="s">
         <v>154</v>
       </c>
@@ -3762,7 +3817,7 @@
         <v>1939</v>
       </c>
     </row>
-    <row r="36" spans="1:11">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A36" s="1" t="s">
         <v>155</v>
       </c>
@@ -3773,7 +3828,7 @@
         <v>-196453</v>
       </c>
     </row>
-    <row r="37" spans="1:11">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A37" s="1" t="s">
         <v>156</v>
       </c>
@@ -3802,7 +3857,7 @@
         <v>1736</v>
       </c>
     </row>
-    <row r="38" spans="1:11">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A38" s="1" t="s">
         <v>157</v>
       </c>
@@ -3828,7 +3883,7 @@
         <v>-3563</v>
       </c>
     </row>
-    <row r="39" spans="1:11">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A39" s="1" t="s">
         <v>158</v>
       </c>
@@ -3851,7 +3906,7 @@
         <v>125125</v>
       </c>
     </row>
-    <row r="40" spans="1:11">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A40" s="1" t="s">
         <v>159</v>
       </c>
@@ -3859,7 +3914,7 @@
         <v>3038</v>
       </c>
     </row>
-    <row r="41" spans="1:11">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A41" s="1" t="s">
         <v>160</v>
       </c>
@@ -3867,12 +3922,12 @@
         <v>6968</v>
       </c>
     </row>
-    <row r="42" spans="1:11">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A42" s="1" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="43" spans="1:11">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A43" s="1" t="s">
         <v>162</v>
       </c>
@@ -3889,7 +3944,7 @@
         <v>-94681</v>
       </c>
     </row>
-    <row r="44" spans="1:11">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A44" s="1" t="s">
         <v>163</v>
       </c>
@@ -3903,7 +3958,7 @@
         <v>-247627</v>
       </c>
     </row>
-    <row r="45" spans="1:11">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A45" s="1" t="s">
         <v>164</v>
       </c>
@@ -3914,7 +3969,7 @@
         <v>3094</v>
       </c>
     </row>
-    <row r="46" spans="1:11">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A46" s="1" t="s">
         <v>165</v>
       </c>
@@ -3925,7 +3980,7 @@
         <v>-74168</v>
       </c>
     </row>
-    <row r="47" spans="1:11">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A47" s="1" t="s">
         <v>166</v>
       </c>
@@ -3933,7 +3988,7 @@
         <v>-7000</v>
       </c>
     </row>
-    <row r="48" spans="1:11">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A48" s="1" t="s">
         <v>167</v>
       </c>
@@ -3941,7 +3996,7 @@
         <v>-427</v>
       </c>
     </row>
-    <row r="49" spans="1:11">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A49" s="1" t="s">
         <v>168</v>
       </c>
@@ -3976,7 +4031,7 @@
         <v>-190452</v>
       </c>
     </row>
-    <row r="50" spans="1:11">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A50" s="1" t="s">
         <v>169</v>
       </c>
@@ -3987,7 +4042,7 @@
         <v>5469</v>
       </c>
     </row>
-    <row r="51" spans="1:11">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A51" s="1" t="s">
         <v>170</v>
       </c>
@@ -4004,7 +4059,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="52" spans="1:11">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A52" s="1" t="s">
         <v>171</v>
       </c>
@@ -4027,7 +4082,7 @@
         <v>-33113</v>
       </c>
     </row>
-    <row r="53" spans="1:11">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A53" s="1" t="s">
         <v>172</v>
       </c>
@@ -4044,7 +4099,7 @@
         <v>-157964</v>
       </c>
     </row>
-    <row r="54" spans="1:11">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A54" s="1" t="s">
         <v>173</v>
       </c>
@@ -4058,7 +4113,7 @@
         <v>3786</v>
       </c>
     </row>
-    <row r="55" spans="1:11">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A55" s="1" t="s">
         <v>174</v>
       </c>
@@ -4072,7 +4127,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="56" spans="1:11">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A56" s="1" t="s">
         <v>175</v>
       </c>
@@ -4080,12 +4135,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:11">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A57" s="1" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="58" spans="1:11">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A58" s="1" t="s">
         <v>177</v>
       </c>
@@ -4108,7 +4163,7 @@
         <v>6314</v>
       </c>
     </row>
-    <row r="59" spans="1:11">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A59" s="1" t="s">
         <v>178</v>
       </c>
@@ -4143,7 +4198,7 @@
         <v>14977</v>
       </c>
     </row>
-    <row r="60" spans="1:11">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A60" s="1" t="s">
         <v>179</v>
       </c>
@@ -4178,7 +4233,7 @@
         <v>-1067</v>
       </c>
     </row>
-    <row r="61" spans="1:11">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A61" s="1" t="s">
         <v>180</v>
       </c>
@@ -4213,7 +4268,7 @@
         <v>-1122457</v>
       </c>
     </row>
-    <row r="62" spans="1:11">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A62" s="1" t="s">
         <v>181</v>
       </c>
@@ -4224,7 +4279,7 @@
         <v>-8971</v>
       </c>
     </row>
-    <row r="63" spans="1:11">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A63" s="1" t="s">
         <v>182</v>
       </c>
@@ -4232,7 +4287,7 @@
         <v>-112257</v>
       </c>
     </row>
-    <row r="64" spans="1:11">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A64" s="1" t="s">
         <v>183</v>
       </c>
@@ -4243,7 +4298,7 @@
         <v>1710143</v>
       </c>
     </row>
-    <row r="65" spans="1:11">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A65" s="1" t="s">
         <v>184</v>
       </c>
@@ -4257,7 +4312,7 @@
         <v>-80000</v>
       </c>
     </row>
-    <row r="66" spans="1:11">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A66" s="1" t="s">
         <v>185</v>
       </c>
@@ -4265,7 +4320,7 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="67" spans="1:11">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A67" s="1" t="s">
         <v>186</v>
       </c>
@@ -4279,7 +4334,7 @@
         <v>-1493</v>
       </c>
     </row>
-    <row r="68" spans="1:11">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A68" s="1" t="s">
         <v>187</v>
       </c>
@@ -4287,7 +4342,7 @@
         <v>-163846</v>
       </c>
     </row>
-    <row r="69" spans="1:11">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A69" s="1" t="s">
         <v>188</v>
       </c>
@@ -4304,7 +4359,7 @@
         <v>-133984</v>
       </c>
     </row>
-    <row r="70" spans="1:11">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A70" s="1" t="s">
         <v>189</v>
       </c>
@@ -4324,7 +4379,7 @@
         <v>217417</v>
       </c>
     </row>
-    <row r="71" spans="1:11">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A71" s="1" t="s">
         <v>190</v>
       </c>
@@ -4344,7 +4399,7 @@
         <v>286958</v>
       </c>
     </row>
-    <row r="72" spans="1:11">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A72" s="1" t="s">
         <v>191</v>
       </c>
@@ -4376,7 +4431,7 @@
         <v>-993250</v>
       </c>
     </row>
-    <row r="73" spans="1:11">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A73" s="1" t="s">
         <v>192</v>
       </c>
@@ -4405,7 +4460,7 @@
         <v>300000</v>
       </c>
     </row>
-    <row r="74" spans="1:11">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A74" s="1" t="s">
         <v>193</v>
       </c>
@@ -4416,7 +4471,7 @@
         <v>34562</v>
       </c>
     </row>
-    <row r="75" spans="1:11">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A75" s="1" t="s">
         <v>194</v>
       </c>
@@ -4433,7 +4488,7 @@
         <v>29888</v>
       </c>
     </row>
-    <row r="76" spans="1:11">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A76" s="1" t="s">
         <v>195</v>
       </c>
@@ -4450,7 +4505,7 @@
         <v>31924</v>
       </c>
     </row>
-    <row r="77" spans="1:11">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A77" s="1" t="s">
         <v>196</v>
       </c>
@@ -4476,7 +4531,7 @@
         <v>-49765</v>
       </c>
     </row>
-    <row r="78" spans="1:11">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A78" s="1" t="s">
         <v>197</v>
       </c>
@@ -4484,7 +4539,7 @@
         <v>-969</v>
       </c>
     </row>
-    <row r="79" spans="1:11">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A79" s="1" t="s">
         <v>198</v>
       </c>
@@ -4510,7 +4565,7 @@
         <v>-408186</v>
       </c>
     </row>
-    <row r="80" spans="1:11">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A80" s="1" t="s">
         <v>199</v>
       </c>
@@ -4527,7 +4582,7 @@
         <v>350384</v>
       </c>
     </row>
-    <row r="81" spans="1:11">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A81" s="1" t="s">
         <v>200</v>
       </c>
@@ -4544,7 +4599,7 @@
         <v>259994</v>
       </c>
     </row>
-    <row r="82" spans="1:11">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A82" s="1" t="s">
         <v>201</v>
       </c>
@@ -4561,7 +4616,7 @@
         <v>6373</v>
       </c>
     </row>
-    <row r="83" spans="1:11">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A83" s="1" t="s">
         <v>202</v>
       </c>
@@ -4572,7 +4627,7 @@
         <v>-52777</v>
       </c>
     </row>
-    <row r="84" spans="1:11">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A84" s="1" t="s">
         <v>203</v>
       </c>
@@ -4586,7 +4641,7 @@
         <v>26860</v>
       </c>
     </row>
-    <row r="85" spans="1:11">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A85" s="1" t="s">
         <v>204</v>
       </c>
@@ -4597,7 +4652,7 @@
         <v>-6223</v>
       </c>
     </row>
-    <row r="86" spans="1:11">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A86" s="1" t="s">
         <v>205</v>
       </c>
@@ -4605,7 +4660,7 @@
         <v>484368</v>
       </c>
     </row>
-    <row r="87" spans="1:11">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A87" s="1" t="s">
         <v>206</v>
       </c>
@@ -4613,12 +4668,12 @@
         <v>350384</v>
       </c>
     </row>
-    <row r="88" spans="1:11">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A88" s="1" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="89" spans="1:11">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A89" s="1" t="s">
         <v>208</v>
       </c>
@@ -4653,7 +4708,7 @@
         <v>58847</v>
       </c>
     </row>
-    <row r="90" spans="1:11">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A90" s="1" t="s">
         <v>209</v>
       </c>
@@ -4688,17 +4743,17 @@
         <v>90146</v>
       </c>
     </row>
-    <row r="91" spans="1:11">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A91" s="1" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="92" spans="1:11">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A92" s="1" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="93" spans="1:11">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A93" s="1" t="s">
         <v>212</v>
       </c>
@@ -4721,7 +4776,7 @@
         <v>9907</v>
       </c>
     </row>
-    <row r="94" spans="1:11">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A94" s="1" t="s">
         <v>213</v>
       </c>
@@ -4738,7 +4793,7 @@
         <v>3033</v>
       </c>
     </row>
-    <row r="95" spans="1:11">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A95" s="1" t="s">
         <v>214</v>
       </c>

</xml_diff>